<commit_message>
update pageViews & drawProteins
</commit_message>
<xml_diff>
--- a/data/pageViews.xlsx
+++ b/data/pageViews.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8900" yWindow="0" windowWidth="25600" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E31" sqref="E30:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -569,6 +570,89 @@
       <c r="B21">
         <v>5817</v>
       </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10051</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B23">
+        <v>8004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B24">
+        <v>6080</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B25">
+        <v>6444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B26">
+        <v>5994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B27">
+        <v>5598</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B28">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B29">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B30">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B31">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>